<commit_message>
E2e test cases added
</commit_message>
<xml_diff>
--- a/Test1/resources/MariottInputs.xlsx
+++ b/Test1/resources/MariottInputs.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/vid/New/AT_Kavya/Test1/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE19D158-1867-DB48-A506-A057338EE9B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596C4CFB-8162-6641-84E4-3395ED043263}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{0CDFBA3E-5718-8841-ABD6-9CDBD1D8F275}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{0CDFBA3E-5718-8841-ABD6-9CDBD1D8F275}"/>
   </bookViews>
   <sheets>
-    <sheet name="BookNow" sheetId="1" r:id="rId1"/>
-    <sheet name="Find&amp;Reserve" sheetId="4" r:id="rId2"/>
+    <sheet name="HomePage" sheetId="1" r:id="rId1"/>
+    <sheet name="SingnInPage" sheetId="4" r:id="rId2"/>
     <sheet name="Special" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -77,9 +77,6 @@
     <t>24/01/2021</t>
   </si>
   <si>
-    <t>2Room</t>
-  </si>
-  <si>
     <t>2 Adults Per Room</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Coorg, Karnataka, India</t>
+  </si>
+  <si>
+    <t>2 Rooms</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,16 +548,16 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -565,7 +565,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -574,16 +574,16 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Rest Assured codes added
</commit_message>
<xml_diff>
--- a/Test1/resources/MariottInputs.xlsx
+++ b/Test1/resources/MariottInputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/vid/New/AT_Kavya/Test1/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596C4CFB-8162-6641-84E4-3395ED043263}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B138533-B964-034E-8BC5-285B981D6504}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{0CDFBA3E-5718-8841-ABD6-9CDBD1D8F275}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{0CDFBA3E-5718-8841-ABD6-9CDBD1D8F275}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Control Flag</t>
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Destination</t>
@@ -493,7 +490,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,25 +510,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -539,51 +536,51 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>